<commit_message>
Fix Excel file - corrected amortization NaN values
</commit_message>
<xml_diff>
--- a/operaciones.xlsx
+++ b/operaciones.xlsx
@@ -635,8 +635,12 @@
           <t>b</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
       <c r="G7" t="n">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Fix Monto Invertido calculation to include initial positions
- Add logic to calculate value of positions at start of selected period
- Include initial invested amount proportional to remaining nominals
- Fix issue where assets purchased before period start showed -- invested
- Add backup file for safety
- Update operaciones.xlsx with latest data

The Monto Invertido now correctly shows:
- Initial positions value (proportional to final nominals)
- Plus purchases during period
- Minus sales during period
</commit_message>
<xml_diff>
--- a/operaciones.xlsx
+++ b/operaciones.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29325"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5FC95BC-B647-4F93-8021-FDB664F19479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A1B662B-C556-4F51-A514-9863D4D73A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="63">
   <si>
     <t>Fecha</t>
   </si>
@@ -598,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -755,7 +755,7 @@
         <v>12</v>
       </c>
       <c r="G5">
-        <v>750</v>
+        <v>375</v>
       </c>
       <c r="M5" t="s">
         <v>18</v>
@@ -805,14 +805,14 @@
         <v>12</v>
       </c>
       <c r="E7">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="F7">
         <v>68.5</v>
       </c>
       <c r="G7">
         <f>+F7*E7</f>
-        <v>34250</v>
+        <v>68500</v>
       </c>
       <c r="M7" t="s">
         <v>25</v>
@@ -823,10 +823,10 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="1">
-        <v>45846</v>
+        <v>45698</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -834,11 +834,15 @@
       <c r="D8" t="s">
         <v>12</v>
       </c>
+      <c r="E8">
+        <v>200</v>
+      </c>
+      <c r="F8">
+        <v>64.7</v>
+      </c>
       <c r="G8">
-        <v>8000</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>27</v>
+        <f>+F8*E8</f>
+        <v>12940</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -846,7 +850,7 @@
         <v>45846</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -855,11 +859,10 @@
         <v>12</v>
       </c>
       <c r="G9">
-        <v>750</v>
-      </c>
-      <c r="J9" s="3"/>
+        <v>1600</v>
+      </c>
       <c r="Q9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -873,90 +876,108 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10">
+        <v>75</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="Q10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="1">
+        <v>45846</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
         <v>15</v>
       </c>
-      <c r="G10">
+      <c r="G11">
         <f>1575/2</f>
         <v>787.5</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q11" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="1"/>
-      <c r="Q11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="1"/>
       <c r="Q12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="1"/>
       <c r="Q13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="1"/>
       <c r="Q14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="1"/>
       <c r="Q15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="1"/>
       <c r="Q16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="1"/>
       <c r="Q17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="1"/>
       <c r="Q18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="1"/>
       <c r="Q19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="1"/>
       <c r="Q20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="1"/>
       <c r="Q21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="1"/>
       <c r="Q22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="1"/>
+      <c r="Q23" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="1"/>
@@ -973,25 +994,28 @@
     <row r="28" spans="1:17">
       <c r="A28" s="1"/>
     </row>
+    <row r="29" spans="1:17">
+      <c r="A29" s="1"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G9">
-    <sortCondition ref="A2:A9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G10">
+    <sortCondition ref="A2:A10"/>
   </sortState>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{9837364A-ACA4-4040-937F-F0F8B099CD79}">
-      <formula1>$M$1:$M$9</formula1>
+      <formula1>$M$1:$M$10</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{5ACDAC43-0A2C-44ED-89F3-6CC7CBBC5473}">
       <formula1>$O$1:$O$7</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1" xr:uid="{072F3766-733D-4D00-B107-5AF1B31BCE79}">
-      <formula1>$Q$1:$Q$26</formula1>
+      <formula1>$Q$1:$Q$27</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6 B8:B28" xr:uid="{D82FC90E-F4C1-4FEE-90A7-1E7B4FF2C652}">
-      <formula1>$M$1:$M$14</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6 B8:B29" xr:uid="{D82FC90E-F4C1-4FEE-90A7-1E7B4FF2C652}">
+      <formula1>$M$1:$M$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D33" xr:uid="{ED8D13E1-2439-4B9C-AEC1-F990B45E5811}">
-      <formula1>$Q$1:$Q$48</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D34" xr:uid="{ED8D13E1-2439-4B9C-AEC1-F990B45E5811}">
+      <formula1>$Q$1:$Q$49</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1002,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AE11B3-0E9A-43BD-8421-E8F835D75104}">
   <dimension ref="A1:Z236"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>